<commit_message>
several changes to the excel file - added a new Test sheet to test out functionality
</commit_message>
<xml_diff>
--- a/skolske zvonenie.xlsx
+++ b/skolske zvonenie.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylar\PycharmProjects\math teaching related\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\NoahBennet\school_bell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A553F8D7-3338-4EF6-A99F-2A868B9CF995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D61C319-6B4A-4206-BD56-902EDD577A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51BE0B57-5BA1-4DA8-8E01-0B8897123499}"/>
   </bookViews>
   <sheets>
     <sheet name="Rozvrh" sheetId="1" r:id="rId1"/>
     <sheet name="Zvonenie" sheetId="3" r:id="rId2"/>
-    <sheet name="Data" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Test" sheetId="4" r:id="rId3"/>
+    <sheet name="Data" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>Pondelok</t>
   </si>
@@ -169,7 +170,22 @@
     <t>áno iba pred koncom hodiny</t>
   </si>
   <si>
-    <t>Na liste Zvonenie si môžete zmeniť časy jednotlivých zvonení.</t>
+    <t>Hlasitosť zvonenia</t>
+  </si>
+  <si>
+    <t>Po zmene nejakej hodnoty je potrebné uložiť súbor a program zavrieť a znovu spustiť.</t>
+  </si>
+  <si>
+    <t>Na hárke Zvonenie si môžete zmeniť časy jednotlivých zvonení, ako aj hlasitosť zvonenia.</t>
+  </si>
+  <si>
+    <t>áno</t>
+  </si>
+  <si>
+    <t>Okrem zadaných časov zvoniť sa má každý deň aj o:</t>
+  </si>
+  <si>
+    <t>Chcem otestovať zvonenie</t>
   </si>
 </sst>
 </file>
@@ -406,18 +422,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -473,32 +479,59 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="1"/>
     </xf>
@@ -506,7 +539,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -861,331 +904,345 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="9.140625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="9.140625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="7">
+      <c r="A2" s="18"/>
+      <c r="B2" s="4">
         <f>Zvonenie!$B2</f>
         <v>0.3263888888888889</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="5">
         <f>Zvonenie!$B3</f>
         <v>0.36458333333333331</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="5">
         <f>Zvonenie!$B4</f>
         <v>0.40277777777777773</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="5">
         <f>Zvonenie!$B5</f>
         <v>0.44791666666666669</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="5">
         <f>Zvonenie!$B6</f>
         <v>0.4861111111111111</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="5">
         <f>Zvonenie!$B7</f>
         <v>0.52430555555555558</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="5">
         <f>Zvonenie!$B8</f>
         <v>0.55902777777777779</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="5">
         <f>Zvonenie!$B9</f>
         <v>0.59375</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="5">
         <f>Zvonenie!$B10</f>
         <v>0.62847222222222221</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="9">
+      <c r="A3" s="19"/>
+      <c r="B3" s="6">
         <f>Zvonenie!$C2</f>
         <v>0.3576388888888889</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <f>Zvonenie!$C3</f>
         <v>0.39583333333333331</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <f>Zvonenie!$C4</f>
         <v>0.43402777777777773</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="7">
         <f>Zvonenie!$C5</f>
         <v>0.47916666666666669</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <f>Zvonenie!$C6</f>
         <v>0.51736111111111105</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="7">
         <f>Zvonenie!$C7</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="7">
         <f>Zvonenie!$C8</f>
         <v>0.59027777777777779</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="7">
         <f>Zvonenie!$C9</f>
         <v>0.625</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="7">
         <f>Zvonenie!$C10</f>
         <v>0.65972222222222221</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="13" t="s">
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="16" t="s">
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="16" t="s">
+      <c r="C6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="16" t="s">
+      <c r="B7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="16" t="s">
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="25" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="17">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="17">
-        <v>1</v>
-      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="A15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="6">
-    <mergeCell ref="A15:F15"/>
+  <mergeCells count="7">
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A1:A3"/>
@@ -1193,13 +1250,13 @@
     <mergeCell ref="D10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:J8">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"zvoniť iba na konci"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"zvoniť iba na začiatku"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"zvoniť"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1242,135 +1299,220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD3112E-405F-4934-A6B7-D7BEA4FB06CA}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="23"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="25">
         <v>0.3263888888888889</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="25">
         <v>0.3576388888888889</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="25">
         <v>0.36458333333333331</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="25">
         <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="25">
         <v>0.40277777777777773</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="25">
         <v>0.43402777777777773</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="25">
         <v>0.44791666666666669</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="25">
         <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="25">
         <v>0.4861111111111111</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="25">
         <v>0.51736111111111105</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="25">
         <v>0.52430555555555558</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="25">
         <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="25">
         <v>0.55902777777777779</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="25">
         <v>0.59027777777777779</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="25">
         <v>0.59375</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="25">
         <v>0.625</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="25">
         <v>0.62847222222222221</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="25">
         <v>0.65972222222222221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="26">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nesprávna hodnota" error="Hodnota tejto bunky musí byť celé číslo medzi 1 a 100." promptTitle="Hlasitosť v %" prompt="Hlasitosť zvonenia je udávaná v percentách. Daná hodnota musí byť celé číslo medzi 1 a 100. Odporúčaná hodnota: 20." sqref="C12" xr:uid="{DD068B64-C53E-4D4B-A935-DF4B61C0FD5B}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC75641-C88E-4788-823B-146D93D78085}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A2:F2">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$D$1="áno"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>$D$1="nie"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nesprávna hodnota" error="Vyberte jednu z možností áno / nie." xr:uid="{661F162A-D5A9-4926-A6EF-E918B42EDAD3}">
+          <x14:formula1>
+            <xm:f>Data!$A$11:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80401F6-DD24-487C-A2F9-FC0A6C22B193}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,6 +1557,16 @@
         <v>29</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>